<commit_message>
Auto update: 2025-05-20 18:51:56
</commit_message>
<xml_diff>
--- a/relevant_companies.xlsx
+++ b/relevant_companies.xlsx
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -504,24 +504,24 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>07:32:31</t>
+          <t>09:38:51</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FUTURE ENTERPRISES &amp; HOLDING LLP</t>
+          <t>MYSTIC PARTNERS &amp; CO LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>OC456787</t>
+          <t>16460843</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -542,24 +542,24 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>07:32:31</t>
+          <t>08:52:24</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SSMC INVESTMENTS LTD</t>
+          <t>DANCRAFT LLP</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16461213</t>
+          <t>OC456792</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -580,24 +580,24 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>09:38:51</t>
+          <t>10:44:26</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>GS GEPE II SIDECAR IV GP LLP</t>
+          <t>MOSU VENTURES LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SO308186</t>
+          <t>16461209</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -618,24 +618,24 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>05:39:32</t>
+          <t>09:38:51</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PULSE SUMMIT CAPITAL LTD</t>
+          <t>GLOBAL SQUARE INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16461206</t>
+          <t>16460615</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -656,24 +656,24 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>09:38:51</t>
+          <t>07:32:31</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>HAYES PARTNERS LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16460412</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -694,24 +694,24 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>14:43:22</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -732,24 +732,24 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>14:43:22</t>
+          <t>06:52:20</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>KVP VENTURES LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16460424</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -770,24 +770,24 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>14:43:22</t>
+          <t>06:52:20</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -808,24 +808,24 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>14:43:22</t>
+          <t>07:32:31</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DELWAR INVESTMENTS LIMITED</t>
+          <t>PULSE SUMMIT CAPITAL LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16460585</t>
+          <t>16461206</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -846,24 +846,24 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>07:32:31</t>
+          <t>09:38:51</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>GS GEPE II SIDECAR IV GP LLP</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>SO308186</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -884,24 +884,24 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>09:38:51</t>
+          <t>05:39:32</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>MYSTIC PARTNERS &amp; CO LTD</t>
+          <t>SSMC INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16460843</t>
+          <t>16461213</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -922,24 +922,24 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>08:52:24</t>
+          <t>09:38:51</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>GLOBAL SQUARE INVESTMENTS LTD</t>
+          <t>FUTURE ENTERPRISES &amp; HOLDING LLP</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16460615</t>
+          <t>OC456787</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -965,19 +965,19 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>HAYES PARTNERS LTD</t>
+          <t>DELWAR INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16460412</t>
+          <t>16460585</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -998,24 +998,24 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>05:39:32</t>
+          <t>07:32:31</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>KVP VENTURES LIMITED</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16460424</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1036,24 +1036,24 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>06:52:20</t>
+          <t>14:43:22</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1074,24 +1074,24 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>06:52:20</t>
+          <t>14:43:22</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>MOSU VENTURES LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16461209</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1112,7 +1112,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>09:38:51</t>
+          <t>14:43:22</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>DANCRAFT LLP</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>OC456792</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1150,24 +1150,24 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>10:44:26</t>
+          <t>14:43:22</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
+          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16457272</t>
+          <t>LP024176</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1193,19 +1193,19 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>NEWCO SWANSEA SOCIAL INFRASTRUCTURE LP</t>
+          <t>DCR HOLDINGS &amp; INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>LP024176</t>
+          <t>16457272</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 20:03:43
</commit_message>
<xml_diff>
--- a/relevant_companies.xlsx
+++ b/relevant_companies.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,19 +509,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,19 +547,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,19 +585,19 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -623,19 +623,19 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,19 +661,19 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -699,19 +699,19 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -738,6 +738,994 @@
       <c r="H8" t="inlineStr">
         <is>
           <t>Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>16456642</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>JJOHN INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>16456276</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>THE REEL MED LLP</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>OC456780</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>KNOTT INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>16458684</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>PONGPONG MALATANG LTD</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>16458077</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-19</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MUSICROOTS LTD</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>16455514</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr"/>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>SIC</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>ESLB INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>16455669</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr"/>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>ECHO VENTURES GROUP LIMITED</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>16455744</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-18</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr"/>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>20:03:42</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Ventures</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>TALKSGPT AI LTD</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>16455313</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr"/>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>GP</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>ARISSA INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>16455197</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SLAM DUNK INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>16455167</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DAVISON FAMILY CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>16455115</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-17</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>GROWTHFORGE MANAGEMENT LLP</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>OC456769</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>TUERNER IMMIGRATION LLP</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>OC456770</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr"/>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>IX PARTNERS LLP</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>OC456771</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-16</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr"/>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>20:03:41</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Partners</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16453716</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr"/>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16453466</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>ALDABBOUS UK INVESTMENTS LTD</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>16453476</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr"/>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Investments</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16453733</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr"/>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Partners</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>GOLDEN VENTURES LONDON LTD</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>16452104</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-05-15</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr"/>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Ventures</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SYNERGY FUNDING LTD</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>16449538</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr"/>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Fund</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>ATHENA PARTNERSHIP LTD</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>16449517</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr"/>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Partners</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16449512</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr"/>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>FROST CAPITAL LTD</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>16450073</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-05-14</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr"/>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>20:03:40</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Capital</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>OVERSEAS STUDY HELPLINE LTD</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>16443154</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr"/>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>20:03:38</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>LP</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BRICK &amp; BEAM VENTURES LTD</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16443239</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-05-12</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>active</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr"/>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>2025-05-20</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>20:03:38</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Ventures</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto update: 2025-05-20 20:07:55
</commit_message>
<xml_diff>
--- a/relevant_companies.xlsx
+++ b/relevant_companies.xlsx
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,19 +509,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,19 +547,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -623,19 +623,19 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,19 +661,19 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -699,19 +699,19 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
+          <t>KNOTT INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16456642</t>
+          <t>16458684</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JJOHN INVESTMENTS LIMITED</t>
+          <t>THE REEL MED LLP</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16456276</t>
+          <t>OC456780</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -813,19 +813,19 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>THE REEL MED LLP</t>
+          <t>PONGPONG MALATANG LTD</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OC456780</t>
+          <t>16458077</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -851,19 +851,19 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KNOTT INVESTMENTS LIMITED</t>
+          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16458684</t>
+          <t>16456642</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -896,12 +896,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>PONGPONG MALATANG LTD</t>
+          <t>JJOHN INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16458077</t>
+          <t>16456276</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -927,19 +927,19 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MUSICROOTS LTD</t>
+          <t>ECHO VENTURES GROUP LIMITED</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16455514</t>
+          <t>16455744</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ECHO VENTURES GROUP LIMITED</t>
+          <t>MUSICROOTS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16455744</t>
+          <t>16455514</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>SIC</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TALKSGPT AI LTD</t>
+          <t>DAVISON FAMILY CAPITAL LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16455313</t>
+          <t>16455115</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>SLAM DUNK INVESTMENTS LTD</t>
+          <t>TALKSGPT AI LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16455167</t>
+          <t>16455313</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1155,19 +1155,19 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DAVISON FAMILY CAPITAL LTD</t>
+          <t>SLAM DUNK INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>16455115</t>
+          <t>16455167</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1193,19 +1193,19 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GROWTHFORGE MANAGEMENT LLP</t>
+          <t>IX PARTNERS LLP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OC456769</t>
+          <t>OC456771</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1231,7 +1231,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IX PARTNERS LLP</t>
+          <t>GROWTHFORGE MANAGEMENT LLP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OC456771</t>
+          <t>OC456769</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1307,19 +1307,19 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
+          <t>GOLDEN VENTURES LONDON LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16453716</t>
+          <t>16452104</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1345,19 +1345,19 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
+          <t>ALDABBOUS UK INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16453466</t>
+          <t>16453476</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ALDABBOUS UK INVESTMENTS LTD</t>
+          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16453476</t>
+          <t>16453466</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
+          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16453733</t>
+          <t>16453716</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1459,19 +1459,19 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GOLDEN VENTURES LONDON LTD</t>
+          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16452104</t>
+          <t>16453733</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SYNERGY FUNDING LTD</t>
+          <t>FROST CAPITAL LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16449538</t>
+          <t>16450073</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1535,7 +1535,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>Fund</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
+          <t>SYNERGY FUNDING LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16449512</t>
+          <t>16449538</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1611,19 +1611,19 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Fund</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FROST CAPITAL LTD</t>
+          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16450073</t>
+          <t>16449512</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-20 20:13:18
</commit_message>
<xml_diff>
--- a/relevant_companies.xlsx
+++ b/relevant_companies.xlsx
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DGPI LTD</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>SC849118</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,19 +509,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,19 +547,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -592,12 +592,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>DGPI LTD</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>SC849118</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -623,19 +623,19 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,19 +661,19 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -699,19 +699,19 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KNOTT INVESTMENTS LIMITED</t>
+          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16458684</t>
+          <t>16456642</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -782,12 +782,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>THE REEL MED LLP</t>
+          <t>JJOHN INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>OC456780</t>
+          <t>16456276</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -813,19 +813,19 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>PONGPONG MALATANG LTD</t>
+          <t>THE REEL MED LLP</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16458077</t>
+          <t>OC456780</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -851,19 +851,19 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
+          <t>PONGPONG MALATANG LTD</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16456642</t>
+          <t>16458077</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -889,19 +889,19 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>JJOHN INVESTMENTS LIMITED</t>
+          <t>KNOTT INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16456276</t>
+          <t>16458684</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ECHO VENTURES GROUP LIMITED</t>
+          <t>MUSICROOTS LTD</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16455744</t>
+          <t>16455514</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>SIC</t>
         </is>
       </c>
     </row>
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MUSICROOTS LTD</t>
+          <t>ECHO VENTURES GROUP LIMITED</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16455514</t>
+          <t>16455744</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>DAVISON FAMILY CAPITAL LTD</t>
+          <t>TALKSGPT AI LTD</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16455115</t>
+          <t>16455313</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1079,7 +1079,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
@@ -1124,12 +1124,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>TALKSGPT AI LTD</t>
+          <t>DAVISON FAMILY CAPITAL LTD</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16455313</t>
+          <t>16455115</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1155,7 +1155,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IX PARTNERS LLP</t>
+          <t>GROWTHFORGE MANAGEMENT LLP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OC456771</t>
+          <t>OC456769</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1231,19 +1231,19 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>TUERNER IMMIGRATION LLP</t>
+          <t>IX PARTNERS LLP</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>OC456770</t>
+          <t>OC456771</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1269,19 +1269,19 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>GROWTHFORGE MANAGEMENT LLP</t>
+          <t>TUERNER IMMIGRATION LLP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OC456769</t>
+          <t>OC456770</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>GOLDEN VENTURES LONDON LTD</t>
+          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16452104</t>
+          <t>16453716</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1345,19 +1345,19 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>ALDABBOUS UK INVESTMENTS LTD</t>
+          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16453476</t>
+          <t>16453466</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
+          <t>ALDABBOUS UK INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16453466</t>
+          <t>16453476</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
+          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16453716</t>
+          <t>16453733</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1459,19 +1459,19 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
+          <t>GOLDEN VENTURES LONDON LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16453733</t>
+          <t>16452104</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>FROST CAPITAL LTD</t>
+          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16450073</t>
+          <t>16449512</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1542,12 +1542,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>ATHENA PARTNERSHIP LTD</t>
+          <t>SYNERGY FUNDING LTD</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16449517</t>
+          <t>16449538</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1573,19 +1573,19 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Fund</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SYNERGY FUNDING LTD</t>
+          <t>ATHENA PARTNERSHIP LTD</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16449538</t>
+          <t>16449517</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1611,19 +1611,19 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Fund</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
+          <t>FROST CAPITAL LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16449512</t>
+          <t>16450073</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">

</xml_diff>

<commit_message>
Auto update: 2025-05-20 20:38:52
</commit_message>
<xml_diff>
--- a/relevant_companies.xlsx
+++ b/relevant_companies.xlsx
@@ -478,12 +478,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
+          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16460503</t>
+          <t>SC849117</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -509,19 +509,19 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>SAMVIV PARTNERS LTD</t>
+          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16460672</t>
+          <t>16462880</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -547,19 +547,19 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>4D CAPITAL PROPCO (44) LIMITED</t>
+          <t>AFROSCOT VENTURES LTD</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16461269</t>
+          <t>16462878</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -585,7 +585,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
@@ -630,12 +630,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AFROSCOT VENTURES LTD</t>
+          <t>SAMVIV PARTNERS LTD</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16462878</t>
+          <t>16460672</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -661,19 +661,19 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ST GEORGE CAPITAL (LAND) LIMITED</t>
+          <t>T GILPIN PHYSIO CONSULTANCY LTD</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16462880</t>
+          <t>16460503</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -699,19 +699,19 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>DAVIDSON CAPITAL HOLDINGS LTD</t>
+          <t>4D CAPITAL PROPCO (44) LIMITED</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SC849117</t>
+          <t>16461269</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -744,12 +744,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
+          <t>THE REEL MED LLP</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16456642</t>
+          <t>OC456780</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -775,19 +775,19 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>LP</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>JJOHN INVESTMENTS LIMITED</t>
+          <t>PONGPONG MALATANG LTD</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>16456276</t>
+          <t>16458077</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -813,19 +813,19 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>THE REEL MED LLP</t>
+          <t>KNOTT INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>OC456780</t>
+          <t>16458684</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -851,19 +851,19 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>LP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>PONGPONG MALATANG LTD</t>
+          <t>KC INVESTMENTS &amp; TRADING LIMITED</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16458077</t>
+          <t>16456642</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -889,19 +889,19 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>KNOTT INVESTMENTS LIMITED</t>
+          <t>JJOHN INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16458684</t>
+          <t>16456276</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -934,12 +934,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MUSICROOTS LTD</t>
+          <t>ECHO VENTURES GROUP LIMITED</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16455514</t>
+          <t>16455744</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -965,7 +965,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>SIC</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
@@ -1010,12 +1010,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ECHO VENTURES GROUP LIMITED</t>
+          <t>MUSICROOTS LTD</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16455744</t>
+          <t>16455514</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1041,19 +1041,19 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>SIC</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>TALKSGPT AI LTD</t>
+          <t>ARISSA INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16455313</t>
+          <t>16455197</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1079,19 +1079,19 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>Investments</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>ARISSA INVESTMENTS LIMITED</t>
+          <t>TALKSGPT AI LTD</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16455197</t>
+          <t>16455313</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1117,7 +1117,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>Investments</t>
+          <t>GP</t>
         </is>
       </c>
     </row>
@@ -1200,12 +1200,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GROWTHFORGE MANAGEMENT LLP</t>
+          <t>TUERNER IMMIGRATION LLP</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>OC456769</t>
+          <t>OC456770</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1276,12 +1276,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>TUERNER IMMIGRATION LLP</t>
+          <t>GROWTHFORGE MANAGEMENT LLP</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>OC456770</t>
+          <t>OC456769</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1314,12 +1314,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
+          <t>GOLDEN VENTURES LONDON LTD</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16453716</t>
+          <t>16452104</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1345,19 +1345,19 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Ventures</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
+          <t>ALDABBOUS UK INVESTMENTS LTD</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16453466</t>
+          <t>16453476</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1390,12 +1390,12 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>ALDABBOUS UK INVESTMENTS LTD</t>
+          <t>CAMBRIDGE SOCIAL INVESTMENTS LIMITED</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16453476</t>
+          <t>16453466</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1428,12 +1428,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
+          <t>CAPITAL &amp; CENTRIC (SYNCHRONICITY) LTD</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16453733</t>
+          <t>16453716</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1459,19 +1459,19 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>GOLDEN VENTURES LONDON LTD</t>
+          <t>GULF TRADE AND INVESTMENT ADVANTAGES JOINT PARTNERSHIP LTD</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16452104</t>
+          <t>16453733</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1497,19 +1497,19 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>Ventures</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
+          <t>FROST CAPITAL LTD</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16449512</t>
+          <t>16450073</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1580,12 +1580,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>ATHENA PARTNERSHIP LTD</t>
+          <t>ASSET CAPITAL 44 OPCO LIMITED</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16449517</t>
+          <t>16449512</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -1611,19 +1611,19 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>Partners</t>
+          <t>Capital</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>FROST CAPITAL LTD</t>
+          <t>ATHENA PARTNERSHIP LTD</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16450073</t>
+          <t>16449517</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1649,7 +1649,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>Capital</t>
+          <t>Partners</t>
         </is>
       </c>
     </row>

</xml_diff>